<commit_message>
Update URL tableau de synthèse
</commit_message>
<xml_diff>
--- a/Tableau de synthèse - Epreuve E5.xlsx
+++ b/Tableau de synthèse - Epreuve E5.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\EasyPHP-5.3.6.0\www\portfolio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\EasyPHP-5.3.6.0\www\Portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30FCD796-71D8-4C25-9AF3-0256DAE925DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{118DA005-D328-4264-9540-F14F445EABB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -126,9 +126,6 @@
     <t>Centre de formation : École IRIS – Paris 17ᵉ</t>
   </si>
   <si>
-    <t xml:space="preserve">Adresse URL du portfolio : </t>
-  </si>
-  <si>
     <t xml:space="preserve"> SLAM</t>
   </si>
   <si>
@@ -249,6 +246,9 @@
   </si>
   <si>
     <t>25/11/25 au 13/12/25</t>
+  </si>
+  <si>
+    <t>Adresse URL du portfolio : https://vincentg94.github.io/Portfolio/</t>
   </si>
 </sst>
 </file>
@@ -790,15 +790,51 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -831,42 +867,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1178,8 +1178,8 @@
   </sheetPr>
   <dimension ref="A1:AQ81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="73" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -1192,83 +1192,83 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24" t="s">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="24"/>
+      <c r="H1" s="26"/>
     </row>
     <row r="2" spans="1:43" ht="41" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
     </row>
     <row r="3" spans="1:43" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" s="37"/>
-      <c r="H3" s="43"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="28"/>
+      <c r="H3" s="34"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="41"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="32"/>
       <c r="F4" s="14" t="s">
         <v>8</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H4" s="21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="35"/>
+      <c r="A5" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="46"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="47"/>
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="43" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -1291,15 +1291,15 @@
       </c>
     </row>
     <row r="7" spans="1:43" s="2" customFormat="1" ht="325.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="23"/>
-      <c r="B7" s="32"/>
-      <c r="C7" s="44" t="s">
+      <c r="A7" s="36"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="44" t="s">
+      <c r="D7" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="44" t="s">
+      <c r="E7" s="22" t="s">
         <v>11</v>
       </c>
       <c r="F7" s="8" t="s">
@@ -1348,16 +1348,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="17.649999999999999" x14ac:dyDescent="0.35">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="27"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="39"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1845,16 +1845,16 @@
       <c r="AQ18"/>
     </row>
     <row r="19" spans="1:43" s="2" customFormat="1" ht="17.649999999999999" x14ac:dyDescent="0.35">
-      <c r="A19" s="28" t="s">
+      <c r="A19" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="29"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="30"/>
+      <c r="B19" s="41"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="42"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -1893,20 +1893,20 @@
     </row>
     <row r="20" spans="1:43" s="2" customFormat="1" ht="100.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="45" t="s">
-        <v>28</v>
-      </c>
-      <c r="D20" s="45"/>
-      <c r="E20" s="45"/>
-      <c r="F20" s="45" t="s">
-        <v>28</v>
-      </c>
-      <c r="G20" s="45"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="G20" s="23"/>
       <c r="H20" s="18"/>
       <c r="I20"/>
       <c r="J20"/>
@@ -1946,19 +1946,19 @@
     </row>
     <row r="21" spans="1:43" s="2" customFormat="1" ht="108.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C21" s="46" t="s">
-        <v>28</v>
-      </c>
-      <c r="D21" s="45"/>
-      <c r="E21" s="45"/>
-      <c r="F21" s="45"/>
-      <c r="G21" s="45" t="s">
-        <v>28</v>
+        <v>38</v>
+      </c>
+      <c r="C21" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="23" t="s">
+        <v>27</v>
       </c>
       <c r="H21" s="18"/>
       <c r="I21"/>
@@ -1999,19 +1999,19 @@
     </row>
     <row r="22" spans="1:43" s="2" customFormat="1" ht="100.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" s="46" t="s">
-        <v>28</v>
-      </c>
-      <c r="D22" s="45"/>
-      <c r="E22" s="45"/>
-      <c r="F22" s="45"/>
-      <c r="G22" s="46" t="s">
-        <v>28</v>
+        <v>39</v>
+      </c>
+      <c r="C22" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="24" t="s">
+        <v>27</v>
       </c>
       <c r="H22" s="18"/>
       <c r="I22"/>
@@ -2052,20 +2052,20 @@
     </row>
     <row r="23" spans="1:43" s="2" customFormat="1" ht="114.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" s="45" t="s">
-        <v>28</v>
-      </c>
-      <c r="D23" s="45"/>
-      <c r="E23" s="45"/>
-      <c r="F23" s="45" t="s">
-        <v>28</v>
-      </c>
-      <c r="G23" s="45"/>
+        <v>40</v>
+      </c>
+      <c r="C23" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="G23" s="23"/>
       <c r="H23" s="18"/>
       <c r="I23"/>
       <c r="J23"/>
@@ -2105,20 +2105,20 @@
     </row>
     <row r="24" spans="1:43" s="2" customFormat="1" ht="114.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C24" s="45" t="s">
-        <v>28</v>
-      </c>
-      <c r="D24" s="45" t="s">
-        <v>28</v>
-      </c>
-      <c r="E24" s="45"/>
-      <c r="F24" s="45"/>
-      <c r="G24" s="45"/>
+        <v>41</v>
+      </c>
+      <c r="C24" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E24" s="23"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="23"/>
       <c r="H24" s="18"/>
       <c r="I24"/>
       <c r="J24"/>
@@ -2247,16 +2247,16 @@
       <c r="AQ26"/>
     </row>
     <row r="27" spans="1:43" s="2" customFormat="1" ht="17.649999999999999" x14ac:dyDescent="0.35">
-      <c r="A27" s="28" t="s">
+      <c r="A27" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="B27" s="29"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="29"/>
-      <c r="H27" s="30"/>
+      <c r="B27" s="41"/>
+      <c r="C27" s="41"/>
+      <c r="D27" s="41"/>
+      <c r="E27" s="41"/>
+      <c r="F27" s="41"/>
+      <c r="G27" s="41"/>
+      <c r="H27" s="42"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2295,19 +2295,19 @@
     </row>
     <row r="28" spans="1:43" s="2" customFormat="1" ht="117.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C28" s="45" t="s">
-        <v>28</v>
-      </c>
-      <c r="D28" s="45"/>
-      <c r="E28" s="45"/>
-      <c r="F28" s="45"/>
-      <c r="G28" s="45"/>
-      <c r="H28" s="47"/>
+        <v>42</v>
+      </c>
+      <c r="C28" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="25"/>
       <c r="I28"/>
       <c r="J28"/>
       <c r="K28"/>
@@ -2346,20 +2346,20 @@
     </row>
     <row r="29" spans="1:43" s="2" customFormat="1" ht="95.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C29" s="45" t="s">
-        <v>28</v>
-      </c>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="47" t="s">
-        <v>28</v>
+        <v>43</v>
+      </c>
+      <c r="C29" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="25" t="s">
+        <v>27</v>
       </c>
       <c r="I29"/>
       <c r="J29"/>
@@ -2399,21 +2399,21 @@
     </row>
     <row r="30" spans="1:43" s="2" customFormat="1" ht="97.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45" t="s">
-        <v>28</v>
-      </c>
-      <c r="E30" s="45"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="45" t="s">
-        <v>28</v>
-      </c>
-      <c r="H30" s="47"/>
+        <v>44</v>
+      </c>
+      <c r="C30" s="23"/>
+      <c r="D30" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E30" s="23"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="H30" s="25"/>
       <c r="I30"/>
       <c r="J30"/>
       <c r="K30"/>
@@ -2452,21 +2452,21 @@
     </row>
     <row r="31" spans="1:43" s="2" customFormat="1" ht="112.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="C31" s="45" t="s">
-        <v>28</v>
-      </c>
-      <c r="D31" s="45"/>
-      <c r="E31" s="45"/>
-      <c r="F31" s="45"/>
-      <c r="G31" s="46" t="s">
-        <v>28</v>
-      </c>
-      <c r="H31" s="47"/>
+        <v>45</v>
+      </c>
+      <c r="C31" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31" s="23"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="23"/>
+      <c r="G31" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="H31" s="25"/>
       <c r="I31"/>
       <c r="J31"/>
       <c r="K31"/>
@@ -2505,20 +2505,20 @@
     </row>
     <row r="32" spans="1:43" s="2" customFormat="1" ht="99.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="C32" s="45"/>
-      <c r="D32" s="45"/>
-      <c r="E32" s="45" t="s">
-        <v>28</v>
-      </c>
-      <c r="F32" s="45"/>
-      <c r="G32" s="45"/>
-      <c r="H32" s="47" t="s">
-        <v>28</v>
+        <v>46</v>
+      </c>
+      <c r="C32" s="23"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="F32" s="23"/>
+      <c r="G32" s="23"/>
+      <c r="H32" s="25" t="s">
+        <v>27</v>
       </c>
       <c r="I32"/>
       <c r="J32"/>
@@ -2739,11 +2739,6 @@
     <row r="81" customFormat="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
@@ -2751,6 +2746,11 @@
     <mergeCell ref="A27:H27"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A5:H5"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>